<commit_message>
excel review added + code modify
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MihaiBucur\Desktop\Facultate anul 3\VVSS\Labs\Lab1\VVSS\Docs\Lab01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA4D06B-BB9C-4B88-B5BD-53ACD8E1AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" tabRatio="650" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -12,12 +18,25 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="88">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -116,19 +135,191 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>RequirementsTasks_v01 - line 1</t>
+  </si>
+  <si>
+    <t>Formatul datelor de intrare/cum sunt introduse nu  e specificat. Solutie: specificare(exemplu: json, xml etc.)</t>
+  </si>
+  <si>
+    <t>RequirementsTasks_v01 - line 4-5</t>
+  </si>
+  <si>
+    <t>RequirementsTasks_v01 - line 12-14</t>
+  </si>
+  <si>
+    <t>Cand se modifica/sterge un task, se modifica/sterg si cele repetitive? Solutie: specificare mai buna a stergerii/modificarii unui task.</t>
+  </si>
+  <si>
+    <t>RequirementsTasks_v01 - line 1-2</t>
+  </si>
+  <si>
+    <t>Lipseste specificarea aplicatiei: mobile, web, cross-platform. Solutie: specificam tipul aplicatiei.</t>
+  </si>
+  <si>
+    <t>Definirea incompleta a unui task: ce e un task activ/inactic, un task repetitiv si activ/inactiv inseamna ca si cele care se repeta sunt active/inactive? . Solutie: specificare task activ/inactiv, detaliere mai buna pentru repetarea unui task</t>
+  </si>
+  <si>
+    <t>Ce este o peroana activa, este un tip de user sau un mod de a spune?</t>
+  </si>
+  <si>
+    <t>Bucur Mihai-Alexandru</t>
+  </si>
+  <si>
+    <t>Biro Iulian Marian</t>
+  </si>
+  <si>
+    <t>A03/A04</t>
+  </si>
+  <si>
+    <t>ClassDiagramTasks-01 - Task class</t>
+  </si>
+  <si>
+    <t>Fields si constructori ambiguu - in requirements task e definit ca primind 2 dati si ore de inceput,dar clasa task are doar un field pentru data si unul pentru ore, iar constructorii nu sunt facuti pentru requirements(unul cu o data doar, iar celalalt cu 2 dati si o ora. Ar trebui precizat mai mult de un int si pentur specificarea minutelor.</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numele de clase nu sunt bine atribuite. TaskIO nu respecta denumirea pentru concepte(e o clasa de view, memorare, control?) si NewEdiController(doar EditController, fara New). </t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>Clasa Main are o dependinta de o clasa Service. Main ar trebui sa fie legat de view/controller.</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>Nu exista clase care sa aiba grija de potentialele erori care  pot aparea.</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>Main -&gt; 57 "we"</t>
+  </si>
+  <si>
+    <t>Notificator -&gt; run</t>
+  </si>
+  <si>
+    <t>TaskIO -&gt; ln 61</t>
+  </si>
+  <si>
+    <t>Este misleading. Solutie: modificare window exit</t>
+  </si>
+  <si>
+    <t>While loop fara conditie de incheiere, doar cu exceptie. Solutie: adaugare variabila "isActive"</t>
+  </si>
+  <si>
+    <t>daca nu se repeta la un interval, atunci task-ul nu mai are endtime, este o decizie eronata la if</t>
+  </si>
+  <si>
+    <t>ArrayTaskList, line 140</t>
+  </si>
+  <si>
+    <t>clone should not be overridden</t>
+  </si>
+  <si>
+    <t>metoda suprascrisa exista</t>
+  </si>
+  <si>
+    <t>creare copy constructor</t>
+  </si>
+  <si>
+    <t>ArrayTaskList, line 141</t>
+  </si>
+  <si>
+    <t>shadow variable for the same name "tasks"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variabila shadow nu mai exista </t>
+  </si>
+  <si>
+    <t>variabila shadow exista</t>
+  </si>
+  <si>
+    <t>DataService, line 34 and 41</t>
+  </si>
+  <si>
+    <t>se apela variabila statica din parinte nu copil</t>
+  </si>
+  <si>
+    <t>se apeleaza direct din parinte</t>
+  </si>
+  <si>
+    <t>static base class members should not be accessed via derived types</t>
+  </si>
+  <si>
+    <t>LinkedTaskList, line 135</t>
+  </si>
+  <si>
+    <t>Unused "private" methods should be removed</t>
+  </si>
+  <si>
+    <t>metoda neutilizata existenta</t>
+  </si>
+  <si>
+    <t>a fost stearsa</t>
+  </si>
+  <si>
+    <t>NewEditController, line 90</t>
+  </si>
+  <si>
+    <t>Sections of code should not be commented out</t>
+  </si>
+  <si>
+    <t>cod comentat in functie</t>
+  </si>
+  <si>
+    <t>comentariu sters</t>
+  </si>
+  <si>
+    <t>switch statements should have at least 3 "case" clauses</t>
+  </si>
+  <si>
+    <t>switch prea scurt</t>
+  </si>
+  <si>
+    <t>schimbat switch cu if pentru citirea mai usoara a codului</t>
+  </si>
+  <si>
+    <t>NewEditController, line 80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -302,77 +493,77 @@
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,14 +574,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -428,7 +622,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -500,7 +694,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -673,105 +867,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.41796875" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.89453125" style="6"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="14" t="s">
+      <c r="I3" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="24"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="14" t="s">
+      <c r="I4" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="26"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -781,55 +984,85 @@
       <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -838,7 +1071,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -847,7 +1080,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -856,86 +1089,83 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="12" t="s">
+      <c r="E25" s="15"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="13"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="1"/>
     </row>
   </sheetData>
@@ -953,104 +1183,113 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="22.05078125" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="32.77734375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="22" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I3" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="27"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I4" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="29"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1064,42 +1303,66 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1108,7 +1371,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1117,7 +1380,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1126,7 +1389,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1135,7 +1398,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1144,7 +1407,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1153,7 +1416,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1162,7 +1425,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1171,7 +1434,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1180,7 +1443,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1189,7 +1452,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1198,7 +1461,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1207,7 +1470,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1216,14 +1479,11 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="12" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="13"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="1"/>
     </row>
   </sheetData>
@@ -1241,105 +1501,113 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="26.734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="17" t="s">
+      <c r="I3" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="30"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="17" t="s">
+      <c r="I4" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="32"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1353,33 +1621,51 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1388,7 +1674,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1397,7 +1683,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1406,7 +1692,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1415,7 +1701,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1424,7 +1710,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1433,7 +1719,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1442,7 +1728,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1451,7 +1737,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1460,7 +1746,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1469,7 +1755,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1478,7 +1764,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1487,7 +1773,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1496,7 +1782,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1505,7 +1791,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1514,7 +1800,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1523,7 +1809,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1532,7 +1818,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1541,14 +1827,11 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C32" s="12" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="13"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="1"/>
     </row>
   </sheetData>
@@ -1566,96 +1849,104 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.9453125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.62890625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="26.734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="37.77734375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="17" t="s">
+      <c r="I3" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="17">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="H4" s="18" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I4" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="H5" s="18" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1672,66 +1963,114 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1741,7 +2080,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1751,7 +2090,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1761,7 +2100,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1771,7 +2110,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1781,7 +2120,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1791,7 +2130,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1801,7 +2140,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1811,7 +2150,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1821,7 +2160,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1831,7 +2170,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1841,7 +2180,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1851,7 +2190,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1861,7 +2200,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1871,7 +2210,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1881,16 +2220,13 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C32" s="34" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="19"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>